<commit_message>
fix data - TU
</commit_message>
<xml_diff>
--- a/data_new.xlsx
+++ b/data_new.xlsx
@@ -1010,7 +1010,7 @@
     <t>ảnh 1 kiểu mà hàng 1 kiểu chắc từ h không dám đặt_hàng tiki nữa</t>
   </si>
   <si>
-    <t>mình mua hàng tiki nhiều lần rồi nhưng lần này quá thất_vọng . đặt màu hồng và màu trắng mà giao cho mình hai cái kiểu_dáng sai hoàn_toàn với cái mình đặt . kiểu_dáng sai , vải xấu , đường may xấu , trên tiki là shop ở thành_phố hồ_chí_minh mà hai áo của mình nguồn_gốc là ở kho hà_nội . dịch không giao được thì_thôi , đằng này_khác nào lừa_đảo</t>
+    <t>mình mua hàng tiki nhiều lần rồi nhưng lần này quá thất_vọng . đặt màu hồng và màu trắng mà giao cho mình hai cái kiểu_dáng sai hoàn_toàn với cái size m đặt . kiểu_dáng sai , vải xấu , đường may xấu , trên tiki là shop ở thành_phố hồ_chí_minh mà hai áo của mình nguồn_gốc là ở kho hà_nội . dịch không giao được thì_thôi , đằng này_khác nào lừa_đảo</t>
   </si>
   <si>
     <t>O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,I-DES,O,B-DES,I-DES,O,O,O,O,O,O,B-DES,O,O,O,O,O,O,O,B-DES,O,O,B-DES,B-DES,O,B-DES,I-DES,B-DES,O,O,O,O,O,O,O,O,O,O,B-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O</t>
@@ -1805,7 +1805,7 @@
     <t>O,O,O,B-DES,B-PRI,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O</t>
   </si>
   <si>
-    <t>1 sao vì đặt_hàng trên web nửa tháng vẫn chưa nhận được hàng , thương_hiệu lớn mà làm_ăn sống_nhăn , giao trễ cũng không thèm báo khách 1 tiếng cũng cóc thèm xử_lý , ncl quá tệ bực cái mình mọi_người đừng mua hãng này trên web nha nó không có bên thứ 3 như * * * quản thì nó chẳng coi khách ra cái thể_thống gì</t>
+    <t>1 sao vì đặt_hàng trên web nửa tháng vẫn chưa nhận được hàng , thương_hiệu lớn mà làm_ăn sống_nhăn , giao trễ cũng không thèm báo khách 1 tiếng cũng cóc thèm xử_lý , ncl quá tệ bực cái size m mọi_người đừng mua hãng này trên web nha nó không có bên thứ 3 như * * * quản thì nó chẳng coi khách ra cái thể_thống gì</t>
   </si>
   <si>
     <t>O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O</t>
@@ -4823,7 +4823,7 @@
     <t>O,O,O,B-DES,B-DES,O,O,O,O,O,O,O,O,O</t>
   </si>
   <si>
-    <t>1 sao vì đặt_hàng trên web nửa tháng vẫn chưa nhận được hàng , thương_hiệu lớn mà làm_ăn sống_nhăn , giao trễ cũng không thèm báo khách 1 tiếng cũng cóc thèm xử_lý , nói_chung là quá tệ bực cái mình mọi người đừng mua hãng này trên web nha nó không có bên thứ 3 như * * * quản thì nó chẳng coi khách ra cái thể_thống gì</t>
+    <t>1 sao vì đặt_hàng trên web nửa tháng vẫn chưa nhận được hàng , thương_hiệu lớn mà làm_ăn sống_nhăn , giao trễ cũng không thèm báo khách 1 tiếng cũng cóc thèm xử_lý , nói_chung là quá tệ bực cái size m mọi người đừng mua hãng này trên web nha nó không có bên thứ 3 như * * * quản thì nó chẳng coi khách ra cái thể_thống gì</t>
   </si>
   <si>
     <t>O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O</t>
@@ -5612,7 +5612,7 @@
     <t>O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,I-DES,O,B-DES</t>
   </si>
   <si>
-    <t>sản_phẩm lần này cực_kỳ tệ ! mình đặt áo này lần thứ ba rồi . áo lần này mình đặt màu trắng . cách đây vài tuần mình có đặt 1 áo màu trắng như_vậy rồi , mình cần đặt thêm 1 cái y_chang để mặc giống nhau nhưng không ngờ , với đơn đặt_hàng giống như đợt trước , mình nhận được 1 chiếc áo không " thể chấp_nhận được " . mình có đính kèm ảnh áo bên dưới , nhìn ảnh còn đỡ , nhìn thật các bạn sẽ thấy rất tệ , nét in thì mờ , màu thì đổ xanh lá hết , không hề giống bất_cứ 1 ảnh nào đăng trên tiki cả . có_thể do khâu kiểm_soát chất_lượng bị lỗi , nhưng ít_nhất nếu mình là người bán , mình sẽ không giao chiếc áo như_vậy cho khách_hàng . nhờ Bộ phận . 'chăm_sóc_khách_hàng tiki xem_xét đổi lại cho mình chiếc áo trắng như trên ảnh , cũng là cái mình muốn đặt_hàng . nếu chỉ còn những chiếc áo kém chất_lượng , không giống như trong ảnh giới_thiệu sản_phẩm , thì cho mình trả lại hàng . mong sớm nhận được phản_hồi từ phía tiki .</t>
+    <t>sản_phẩm lần này cực_kỳ tệ ! mình đặt áo này lần thứ ba rồi . áo lần này mình đặt màu trắng . cách đây vài tuần mình có đặt 1 áo màu trắng như_vậy rồi , mình cần đặt thêm 1 cái y_chang để mặc giống nhau nhưng không ngờ , với đơn đặt_hàng giống như đợt trước , mình nhận được 1 chiếc áo không " thể chấp_nhận được " . mình có đính kèm ảnh áo bên dưới , nhìn ảnh còn đỡ , nhìn thật các bạn sẽ thấy rất tệ , nét in thì mờ , màu thì đổ xanh lá hết , không hề giống bất_cứ 1 ảnh nào đăng trên tiki cả . có_thể do khâu kiểm_soát chất_lượng bị lỗi , nhưng ít_nhất nếu mình là người bán , mình sẽ không giao chiếc áo như_vậy cho khách_hàng . nhờ Bộ phận . 'chăm_sóc_khách_hàng tiki xem_xét đổi lại cho mình chiếc áo trắng như trên ảnh , cũng là cái size m muốn đặt_hàng . nếu chỉ còn những chiếc áo kém chất_lượng , không giống như trong ảnh giới_thiệu sản_phẩm , thì cho mình trả lại hàng . mong sớm nhận được phản_hồi từ phía tiki .</t>
   </si>
   <si>
     <t>O,O,O,O,O,O,O,O,B-DES,O,O,O,O,O,O,B-DES,O,O,O,O,B-DES,I-DES,O,O,O,O,O,O,O,O,O,B-DES,B-DES,I-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,I-DES,O,O,O,B-DES,O,O,B-DES,I-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,B-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,O,O,O,B-DES,I-DES,I-DES,I-DES,I-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O</t>
@@ -9269,7 +9269,7 @@
     <t>O,O,O,O,O,B-DES,O,O,O,O,O,B-DES,O,O,O,O,O,O,O,O,O,O,O</t>
   </si>
   <si>
-    <t>không được như mình mong_đợi , vải hơi mềm , mặc vào không lên dáng , không được như cái mình mua ở rosara cũng tầm ấy tiền</t>
+    <t>không được như mình mong_đợi , vải hơi mềm , mặc vào không lên dáng , không được như cái size m mua ở rosara cũng tầm ấy tiền</t>
   </si>
   <si>
     <t>O,O,O,O,O,O,B-DES,O,B-DES,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-PRI</t>
@@ -9953,7 +9953,7 @@
     <t>quần hơi cộc . shiper giao hàng_không điện_thoại nên gửi nhầm . mình phải đi nhận lại hơi xa .</t>
   </si>
   <si>
-    <t>sản_phẩm tạm ổn . không phải gốc nhật như cái mình từng mua . nhưng mặc ổn lắm nhe m . n . mua sài được lắm . lưu_ý . 56-67 nên mua size xl hoi . shop chọn sai xxl dù mình 67 mà_còn thấy hơi rộng .</t>
+    <t>sản_phẩm tạm ổn . không phải gốc nhật như cái size m từng mua . nhưng mặc ổn lắm nhe m . n . mua sài được lắm . lưu_ý . 56-67 nên mua size xl hoi . shop chọn sai xxl dù mình 67 mà_còn thấy hơi rộng .</t>
   </si>
   <si>
     <t>O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,I-DES,O,O,O,O,O,B-DES,O,O,O,O,O,O,B-DES,O</t>
@@ -10820,7 +10820,7 @@
     <t>O,O,O,O,B-DES,B-DES,O,O,O,O,O,B-DES,O,O,O,O,O,B-DES,I-DES,O,O,O,O,O</t>
   </si>
   <si>
-    <t>quần toàn nilon . ai thích giá rẻ mà tiện thì nên mua . với cả 1 cái trong 5 cái mình đặt bị như kiểu mặc vào xong quệt vào tường</t>
+    <t>quần toàn nilon . ai thích giá rẻ mà tiện thì nên mua . với cả 1 cái trong 5 cái size m đặt bị như kiểu mặc vào xong quệt vào tường</t>
   </si>
   <si>
     <t>B-DES,O,B-DES,O,O,O,B-PRI,I-PRI,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O</t>
@@ -11414,7 +11414,7 @@
     <t>B-DES,O,O,O,O,O,O,B-DES,O,O</t>
   </si>
   <si>
-    <t>sản_phẩm tạm ổn . không phải gốc nhật như cái mình từng mua . nhưng mặc ổn lắm nhe m . n . mua sài được lắm . lưu_ý . 56-67 nên mua size xl hoi . shop chọn size xxl dù mình 67 mà_còn thấy hơi rộng .</t>
+    <t>sản_phẩm tạm ổn . không phải gốc nhật như cái size m từng mua . nhưng mặc ổn lắm nhe m . n . mua sài được lắm . lưu_ý . 56-67 nên mua size xl hoi . shop chọn size xxl dù mình 67 mà_còn thấy hơi rộng .</t>
   </si>
   <si>
     <t>O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,O,B-DES,I-DES,O,O,O,O,B-DES,I-DES,O,O,O,O,O,O,B-DES,O</t>
@@ -13778,7 +13778,7 @@
     <t>B-DES,B-DES,B-DES,O,B-DES,O,O,B-DES,O,O,B-DES,O,O,O,O,O,O,B-DES,O,B-DES,O,O</t>
   </si>
   <si>
-    <t>chất_liệu vải thoáng mát , chất_lượng tốt , giao đủ 5 màu mình đặt xl mà tự_nhiên nhận được 4 cái xl 1 cái mình ?</t>
+    <t>chất_liệu vải thoáng mát , chất_lượng tốt , giao đủ 5 màu mình đặt xl mà tự_nhiên nhận được 4 cái xl 1 cái size m ?</t>
   </si>
   <si>
     <t>B-DES,B-DES,O,B-DES,O,O,O,O,O,O,O,B-DES,O,O,B-DES,O,O,O,O,O,O,B-DES,O,O,O,O</t>
@@ -15335,7 +15335,7 @@
     <t>B-DES,B-DES,O,B-DES,B-DES,I-DES,O,O,B-DES,O,O,O</t>
   </si>
   <si>
-    <t>giao nhầm size , mình đặt 10 quần l giao nhầm hai cái sao ,</t>
+    <t>giao nhầm size , mình đặt 10 quần l giao nhầm hai cái size s ,</t>
   </si>
   <si>
     <t>O,O,B-DES,O,O,O,O,B-DES,B-DES,O,O,O,O,O,O</t>

</xml_diff>